<commit_message>
AutoCommit_25 февраля 2024 г. 16:41:13_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:G2"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -832,7 +832,9 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_5 марта 2024 г. 13:46:17_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -500,11 +500,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -776,8 +776,12 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="2">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_12 марта 2024 г. 13:52:00_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -720,8 +720,12 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_19 марта 2024 г. 13:44:56_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -566,9 +566,15 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -664,9 +670,15 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -752,7 +764,9 @@
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2">
+        <v>5</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_26 марта 2024 г. 12:49:49_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -826,8 +826,12 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_16 апреля 2024 г. 12:26:32_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>2ИСИП-722: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>ТК</t>
+  </si>
+  <si>
+    <t>ДЗ_6</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -553,7 +556,9 @@
       <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J2" s="4" t="s">
         <v>35</v>
       </c>
@@ -737,15 +742,27 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K11">
         <v>3</v>
@@ -854,13 +871,21 @@
       <c r="D16" s="2">
         <v>5</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="K16">
         <v>4</v>
@@ -917,15 +942,23 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="2">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K19">
         <v>3</v>
@@ -944,13 +977,21 @@
       <c r="D20" s="2">
         <v>5</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5</v>
+      </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="K20">
         <v>4</v>
@@ -990,13 +1031,17 @@
       <c r="D22" s="2">
         <v>5</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K22">
         <v>4</v>
@@ -1212,15 +1257,21 @@
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="C32" s="2">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K32">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_16 апреля 2024 г. 12:27:18_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -525,7 +525,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -700,15 +700,19 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K9">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_23 апреля 2024 г. 12:21:23_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -522,10 +522,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1250,15 +1250,21 @@
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="C31" s="2">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K31">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_23 апреля 2024 г. 12:25:18_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -522,10 +522,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -936,14 +936,20 @@
       <c r="C18" s="2">
         <v>5</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="2">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K18">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_14 мая 2024 г. 12:14:30_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -522,10 +522,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_14 мая 2024 г. 12:29:30_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -522,10 +522,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -878,22 +878,26 @@
         <v>11</v>
       </c>
       <c r="C14" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F14" s="2">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="K14">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_21 мая 2024 г. 12:35:14_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2ИСИП-722: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>ДЗ_6</t>
+  </si>
+  <si>
+    <t>ДЗ_7</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -197,11 +200,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -213,6 +227,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,10 +539,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -540,7 +557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -559,6 +576,9 @@
       <c r="H2" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="J2" s="4" t="s">
         <v>35</v>
       </c>
@@ -566,7 +586,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -911,7 +931,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="2">
         <v>2</v>
@@ -923,10 +943,12 @@
         <v>2</v>
       </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <v>5</v>
+      </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K15">
         <v>3</v>
@@ -957,9 +979,12 @@
       <c r="H16" s="2">
         <v>5</v>
       </c>
+      <c r="I16" s="5">
+        <v>5</v>
+      </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K16">
         <v>4</v>
@@ -1077,9 +1102,12 @@
       <c r="H20" s="2">
         <v>5</v>
       </c>
+      <c r="I20" s="5">
+        <v>5</v>
+      </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K20">
         <v>4</v>
@@ -1423,11 +1451,15 @@
       <c r="F32" s="2">
         <v>5</v>
       </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="G32" s="2">
+        <v>5</v>
+      </c>
+      <c r="H32" s="2">
+        <v>5</v>
+      </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="K32">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_21 мая 2024 г. 12:37:26_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -934,21 +934,23 @@
         <v>5</v>
       </c>
       <c r="D15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F15" s="2">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
       <c r="H15" s="2">
         <v>5</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="K15">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_21 мая 2024 г. 13:48:16_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -640,13 +640,17 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
       <c r="J5">
         <f t="shared" ref="J5:J32" si="0">SUM(C5:I5)</f>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K5">
         <v>5</v>
@@ -847,13 +851,17 @@
         <v>5</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K12">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_28 мая 2024 г. 12:25:14_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -743,7 +743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -772,7 +772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -780,28 +780,35 @@
         <v>7</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F10" s="2">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="K10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_28 мая 2024 г. 12:30:30_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -722,22 +722,22 @@
         <v>5</v>
       </c>
       <c r="C8" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E8" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F8" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K8">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_4 июня 2024 г. 13:47:58_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -664,22 +664,24 @@
         <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="K6">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_10 июня 2024 г. 11:12:26_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>2ИСИП-722: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -126,16 +126,13 @@
     <t>ДЗ_5</t>
   </si>
   <si>
-    <t>сумма</t>
-  </si>
-  <si>
-    <t>ТК</t>
-  </si>
-  <si>
     <t>ДЗ_6</t>
   </si>
   <si>
     <t>ДЗ_7</t>
+  </si>
+  <si>
+    <t>Лаб_1</t>
   </si>
 </sst>
 </file>
@@ -539,10 +536,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -574,17 +571,15 @@
         <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
@@ -615,13 +610,6 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="J4">
-        <f>SUM(C4:I4)</f>
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -646,13 +634,6 @@
         <v>5</v>
       </c>
       <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J32" si="0">SUM(C5:I5)</f>
-        <v>30</v>
-      </c>
-      <c r="K5">
         <v>5</v>
       </c>
     </row>
@@ -679,13 +660,6 @@
         <v>5</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
     </row>
     <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -708,13 +682,6 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
     </row>
     <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -737,13 +704,6 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
     </row>
     <row r="9" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -766,13 +726,6 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
     </row>
     <row r="10" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -802,13 +755,6 @@
       <c r="I10" s="2">
         <v>5</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
-      </c>
     </row>
     <row r="11" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -835,13 +781,6 @@
       <c r="H11" s="2">
         <v>5</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K11">
-        <v>3</v>
-      </c>
     </row>
     <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -868,13 +807,6 @@
       <c r="H12" s="2">
         <v>5</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K12">
-        <v>5</v>
-      </c>
     </row>
     <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -899,13 +831,6 @@
         <v>5</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="K13">
-        <v>3</v>
-      </c>
     </row>
     <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -932,13 +857,6 @@
       <c r="H14" s="2">
         <v>5</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K14">
-        <v>3</v>
-      </c>
     </row>
     <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -965,13 +883,6 @@
       <c r="H15" s="2">
         <v>5</v>
       </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
     </row>
     <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1001,15 +912,8 @@
       <c r="I16" s="5">
         <v>5</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="K16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1030,15 +934,8 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1059,15 +956,8 @@
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1088,15 +978,8 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1124,15 +1007,8 @@
       <c r="I20" s="5">
         <v>5</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="K20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1153,15 +1029,8 @@
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1182,15 +1051,8 @@
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="J22">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1211,15 +1073,8 @@
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="J23">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="K23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1240,15 +1095,8 @@
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="J24">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1269,15 +1117,8 @@
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1298,15 +1139,8 @@
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1327,15 +1161,8 @@
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="J27">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1356,15 +1183,8 @@
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="J28">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1372,28 +1192,28 @@
         <v>26</v>
       </c>
       <c r="C29" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D29" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E29" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F29" s="2">
-        <v>2</v>
-      </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="J29">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G29" s="2">
+        <v>5</v>
+      </c>
+      <c r="H29" s="2">
+        <v>5</v>
+      </c>
+      <c r="I29" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1414,15 +1234,8 @@
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="J30">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1443,15 +1256,8 @@
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="J31">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="K31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1475,13 +1281,6 @@
       </c>
       <c r="H32" s="2">
         <v>5</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="K32">
-        <v>3</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 11:01:08_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -227,6 +227,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,10 +539,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -913,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -935,7 +938,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -957,7 +960,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -979,7 +982,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1030,7 +1033,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1052,7 +1055,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1074,7 +1077,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1096,7 +1099,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1118,7 +1121,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1140,7 +1143,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1162,7 +1165,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1184,7 +1187,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1213,7 +1216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1235,7 +1238,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1257,7 +1260,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1280,6 +1283,9 @@
         <v>5</v>
       </c>
       <c r="H32" s="2">
+        <v>5</v>
+      </c>
+      <c r="J32" s="6">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 11:24:22_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-722_ТерВер.xlsx
+++ b/_2ИСИП-722_ТерВер.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1191,9 +1191,15 @@
       <c r="H24" s="2">
         <v>5</v>
       </c>
+      <c r="I24" s="5">
+        <v>5</v>
+      </c>
+      <c r="J24" s="6">
+        <v>5</v>
+      </c>
       <c r="L24">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="13" x14ac:dyDescent="0.25">

</xml_diff>